<commit_message>
add support for mac m1
</commit_message>
<xml_diff>
--- a/src/main/java/com/junit/selenium/data/data.xlsx
+++ b/src/main/java/com/junit/selenium/data/data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10509"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5B0DD77-5343-49CC-87DC-B3B0E6FF0B25}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9CA7B39-67CC-174C-AB54-BD05B6F30329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="2880" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2760" yWindow="2880" windowWidth="21600" windowHeight="11380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestSteps" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="31">
   <si>
     <t>TestCase ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -81,65 +81,13 @@
     <t>TS003</t>
   </si>
   <si>
-    <t>输入用户名</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>loginUsernameInputbox</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>TS004</t>
   </si>
   <si>
-    <t>输入密码</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>loginPasswordInptbox</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TS005</t>
-  </si>
-  <si>
-    <t>点击认证按钮</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>loginAuthbtn</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>click</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>TS006</t>
-  </si>
-  <si>
-    <t>选择项目</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>loginProjectlist</t>
-  </si>
-  <si>
-    <t>select</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TS007</t>
-  </si>
-  <si>
-    <t>点击登录</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>loginLoginbtn</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Test Case ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -171,27 +119,27 @@
     <t>PASS</t>
   </si>
   <si>
-    <t>MaoHaonan</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>shellingford1234</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>input</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>5th_test</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Variable</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>FAIL</t>
+  </si>
+  <si>
+    <t>输入信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hello</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>search</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -199,7 +147,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -534,21 +482,20 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="14.5" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="14.25" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="18.375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="27.875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.1640625" collapsed="true"/>
+    <col min="3" max="4" customWidth="true" width="18.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="27.83203125" collapsed="true"/>
     <col min="6" max="6" customWidth="true" width="29.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="9.875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="9.83203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -559,7 +506,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -571,7 +518,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -588,10 +535,10 @@
         <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -608,10 +555,10 @@
         <v>13</v>
       </c>
       <c r="G3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -619,107 +566,44 @@
         <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="G4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="F5" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="G5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
         <v>24</v>
       </c>
-      <c r="C7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" t="s">
-        <v>38</v>
-      </c>
-    </row>
+    </row>
+    <row r="6" spans="1:7"/>
+    <row r="7" spans="1:7"/>
+    <row r="8" spans="1:7"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -735,49 +619,49 @@
       <selection sqref="A1:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="12.5" collapsed="true"/>
-    <col min="2" max="3" customWidth="true" width="12.125" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" width="12.1640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>